<commit_message>
Migrate to PIM 1.7 (#27)
* Update composer.json

* Update doc matching new version

* Update dependency to new pim and new CI

* Migrate to 1.7

* Add Changelog

* Update Jenkinsfile to be able to run CI

* Revert Jenkins file to be able to run on master
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal_EE/init.xlsx
+++ b/src/Resources/fixtures/minimal_EE/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
     <definedName function="false" hidden="false" name="metric_units" vbProcedure="false">metric_units!$B$3:$B$89</definedName>
     <definedName function="false" hidden="false" name="validation_choices" vbProcedure="false">choices!$B$1:$B$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">attributes!$B$6:$AU$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'family main'!$C$5:$AW$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'family main'!$C$5:$Y$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -111,54 +111,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Insert the name of the locales, separated by ",".
-For example : "en_US, fr_FR"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
-For example : 
-jpg, jpeg, png</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
-This should be used for attributes which have a large number of options.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA3" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -182,38 +135,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="Y4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
-For example : 
-jpg, jpeg, png</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
-This should be used for attributes which have a large number of options.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA3" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="400">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -1815,9 +1737,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1827,7 +1749,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6160320" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1860,9 +1782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1872,7 +1794,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6160320" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1910,9 +1832,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>79200</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1922,7 +1844,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5865120" cy="10200600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,9 +1877,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>79200</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1967,7 +1889,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5865120" cy="10200600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2005,9 +1927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2017,7 +1939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6760440" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2050,9 +1972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2062,7 +1984,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6760440" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2096,13 +2018,14 @@
   </sheetPr>
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,7 +2197,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2289,14 +2212,15 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.1122448979592"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="47.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2364,7 +2288,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2379,13 +2303,13 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,7 +2355,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2446,15 +2370,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,7 +2416,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2507,17 +2431,21 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,7 +2527,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2614,14 +2542,15 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3443,7 +3372,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3458,11 +3387,14 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -3497,7 +3429,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3512,15 +3444,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,7 +3570,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3653,15 +3585,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,7 +3711,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3794,15 +3726,15 @@
   </sheetPr>
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4450,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4533,39 +4465,42 @@
   </sheetPr>
   <dimension ref="A1:AV8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="26" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="47" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="49" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4931,7 +4866,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4945,67 +4880,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX7"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="8" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="27" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1000" min="998" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1001" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="0"/>
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="AA1" s="0"/>
-      <c r="AU1" s="0"/>
-      <c r="AV1" s="0"/>
-      <c r="AW1" s="0"/>
-      <c r="AX1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -5014,57 +4925,47 @@
       <c r="B2" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="AA2" s="0"/>
-      <c r="AU2" s="0"/>
-      <c r="AV2" s="0"/>
-      <c r="AW2" s="0"/>
-      <c r="AX2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
     </row>
     <row r="3" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="20" t="s">
+      <c r="C3" s="20" t="s">
         <v>96</v>
       </c>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -5073,79 +4974,7 @@
       <c r="B4" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="V4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA4" s="21" t="s">
+      <c r="C4" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5156,92 +4985,25 @@
       <c r="B5" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="X5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA5" s="22"/>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="C6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
@@ -5251,107 +5013,32 @@
       <c r="T6" s="19"/>
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19"/>
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-      <c r="AL6" s="19"/>
-      <c r="AM6" s="19"/>
-      <c r="AN6" s="19"/>
-      <c r="AO6" s="19"/>
-      <c r="AP6" s="19"/>
-      <c r="AQ6" s="19"/>
-      <c r="AR6" s="19"/>
-      <c r="AS6" s="19"/>
-      <c r="AT6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="AA7" s="6" t="n">
+      <c r="C7" s="6" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:Z3"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T6" type="decimal">
-      <formula1>$P$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N6" type="none">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6:B7 G6:H7 J6:K7 O6:O7 R6:S7" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6:B7" type="list">
       <formula1>boolean_choices</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L6:L7" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6:M7" type="list">
-      <formula1>validation_choices</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:X7 Z6:Z7" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6:AA7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C7" type="list">
       <formula1>boolean_choices</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P6:Q7" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V7" type="list">
-      <formula1>metric_types</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W3:W7" type="list">
-      <formula1>metric_units</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D7" type="list">
-      <formula1>attribute_types</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E7" type="list">
-      <formula1>attribute_groups</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5365,67 +5052,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX6"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="8" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="7" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="27" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1000" min="998" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1001" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="AA1" s="0"/>
-      <c r="AU1" s="0"/>
-      <c r="AV1" s="0"/>
-      <c r="AW1" s="0"/>
-      <c r="AX1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -5434,57 +5097,47 @@
       <c r="B2" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="AA2" s="0"/>
-      <c r="AU2" s="0"/>
-      <c r="AV2" s="0"/>
-      <c r="AW2" s="0"/>
-      <c r="AX2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
     </row>
     <row r="3" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="20" t="s">
+      <c r="C3" s="20" t="s">
         <v>96</v>
       </c>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -5493,79 +5146,7 @@
       <c r="B4" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="V4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA4" s="21" t="s">
+      <c r="C4" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5576,92 +5157,25 @@
       <c r="B5" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="U5" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="X5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA5" s="22"/>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="C6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
@@ -5671,94 +5185,21 @@
       <c r="T6" s="19"/>
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19"/>
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-      <c r="AL6" s="19"/>
-      <c r="AM6" s="19"/>
-      <c r="AN6" s="19"/>
-      <c r="AO6" s="19"/>
-      <c r="AP6" s="19"/>
-      <c r="AQ6" s="19"/>
-      <c r="AR6" s="19"/>
-      <c r="AS6" s="19"/>
-      <c r="AT6" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:Z3"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T6" type="decimal">
-      <formula1>$P$7</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N6" type="none">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6 G6:H6 J6:K6 O6 R6:S6" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6" type="list">
       <formula1>boolean_choices</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L6" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6" type="list">
-      <formula1>validation_choices</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6 Z6" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
       <formula1>boolean_choices</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P6:Q6" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V6" type="list">
-      <formula1>metric_types</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W3:W6" type="list">
-      <formula1>metric_units</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D6" type="list">
-      <formula1>attribute_types</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E6" type="list">
-      <formula1>attribute_groups</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5774,16 +5215,16 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5845,7 +5286,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5860,15 +5301,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5908,7 +5349,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5924,19 +5365,19 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="6" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6011,7 +5452,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6028,15 +5469,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6090,7 +5531,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6106,14 +5547,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6158,7 +5600,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
two locales in EE init file
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal_EE/init.xlsx
+++ b/src/Resources/fixtures/minimal_EE/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
     <definedName function="false" hidden="false" name="metric_types" vbProcedure="false">metric_types!$B$3:$B$11</definedName>
     <definedName function="false" hidden="false" name="metric_units" vbProcedure="false">metric_units!$B$3:$B$89</definedName>
     <definedName function="false" hidden="false" name="validation_choices" vbProcedure="false">choices!$B$1:$B$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">attributes!$B$6:$AU$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">attributes!$B$6:$AV$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'family main'!$C$5:$Y$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
   </definedNames>
@@ -54,7 +54,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X5" authorId="0">
+    <comment ref="Y5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y5" authorId="0">
+    <comment ref="Z5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="408">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -307,6 +307,9 @@
     <t xml:space="preserve">en_US</t>
   </si>
   <si>
+    <t xml:space="preserve">fr_FR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute type</t>
   </si>
   <si>
@@ -382,6 +385,9 @@
     <t xml:space="preserve">label-en_US</t>
   </si>
   <si>
+    <t xml:space="preserve">label-fr_FR</t>
+  </si>
+  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -469,6 +475,9 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
     <t xml:space="preserve">Text</t>
   </si>
   <si>
@@ -484,6 +493,9 @@
     <t xml:space="preserve">Main</t>
   </si>
   <si>
+    <t xml:space="preserve">Catégorie principale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Completeness</t>
   </si>
   <si>
@@ -499,6 +511,9 @@
     <t xml:space="preserve">Second family</t>
   </si>
   <si>
+    <t xml:space="preserve">Deuxième famille</t>
+  </si>
+  <si>
     <t xml:space="preserve">Group properties</t>
   </si>
   <si>
@@ -517,6 +532,9 @@
     <t xml:space="preserve">Other</t>
   </si>
   <si>
+    <t xml:space="preserve">Autres</t>
+  </si>
+  <si>
     <t xml:space="preserve">Option properties</t>
   </si>
   <si>
@@ -556,160 +574,166 @@
     <t xml:space="preserve">tree</t>
   </si>
   <si>
+    <t xml:space="preserve">en_US,fr_FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD,EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPSELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upsell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSTITUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_ADMINISTRATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_CATALOG_MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalog manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog_scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activated</t>
+  </si>
+  <si>
     <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VARIANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X_SELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross sell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPSELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upsell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUBSTITUTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it_support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE_ADMINISTRATOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE_CATALOG_MANAGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalog manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalog_locale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_locale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalog_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default_tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activated</t>
   </si>
   <si>
     <t xml:space="preserve">EUR</t>
@@ -1533,7 +1557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1642,6 +1666,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1737,9 +1773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326520</xdr:colOff>
+      <xdr:colOff>326160</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1749,7 +1785,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6160320" cy="9530280"/>
+          <a:ext cx="6083640" cy="9529920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1782,9 +1818,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>326520</xdr:colOff>
+      <xdr:colOff>326160</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1794,7 +1830,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6160320" cy="9530280"/>
+          <a:ext cx="6083640" cy="9529920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1832,9 +1868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>78840</xdr:colOff>
+      <xdr:colOff>78480</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1844,7 +1880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="5865120" cy="10200600"/>
+          <a:ext cx="5798160" cy="10200240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1877,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>78840</xdr:colOff>
+      <xdr:colOff>78480</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1889,7 +1925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="5865120" cy="10200600"/>
+          <a:ext cx="5798160" cy="10200240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1929,7 +1965,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>326520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1939,7 +1975,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6760440" cy="9530280"/>
+          <a:ext cx="11122200" cy="9829800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1974,7 +2010,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>326520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1984,7 +2020,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6760440" cy="9530280"/>
+          <a:ext cx="11122200" cy="9829800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2018,14 +2054,14 @@
   </sheetPr>
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,7 +2233,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2212,20 +2248,20 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="24.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="47.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="31" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>33</v>
@@ -2233,7 +2269,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>36</v>
@@ -2241,42 +2277,42 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>133</v>
+        <v>139</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>135</v>
+        <v>141</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>137</v>
+        <v>143</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>139</v>
+        <v>145</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2288,7 +2324,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2303,59 +2339,56 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.23"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2370,53 +2403,52 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2431,76 +2463,76 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>36</v>
@@ -2509,16 +2541,16 @@
         <v>36</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -2527,7 +2559,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2542,28 +2574,27 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2571,7 +2602,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2579,7 +2610,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -2587,7 +2618,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2595,7 +2626,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2603,7 +2634,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2611,7 +2642,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2619,7 +2650,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2627,7 +2658,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2635,7 +2666,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2643,7 +2674,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2651,7 +2682,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2659,7 +2690,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2667,7 +2698,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2675,7 +2706,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2683,7 +2714,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2691,7 +2722,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -2699,7 +2730,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2707,7 +2738,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2715,7 +2746,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -2723,7 +2754,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -2731,7 +2762,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -2739,7 +2770,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -2747,7 +2778,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -2755,7 +2786,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -2763,7 +2794,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -2771,7 +2802,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -2779,7 +2810,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -2787,7 +2818,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -2795,7 +2826,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -2803,7 +2834,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -2811,7 +2842,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -2819,7 +2850,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -2827,7 +2858,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -2835,7 +2866,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -2843,7 +2874,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -2851,7 +2882,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -2859,7 +2890,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -2867,7 +2898,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -2875,7 +2906,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -2883,7 +2914,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -2891,7 +2922,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -2899,7 +2930,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -2907,7 +2938,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -2915,7 +2946,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -2923,7 +2954,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -2931,7 +2962,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -2939,7 +2970,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -2947,7 +2978,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -2955,7 +2986,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -2963,7 +2994,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -2971,7 +3002,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -2979,7 +3010,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -2987,7 +3018,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -2995,7 +3026,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -3003,7 +3034,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -3011,7 +3042,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -3019,7 +3050,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -3027,7 +3058,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -3035,7 +3066,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -3043,7 +3074,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3051,7 +3082,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0</v>
@@ -3059,7 +3090,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0</v>
@@ -3067,7 +3098,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0</v>
@@ -3075,7 +3106,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0</v>
@@ -3083,7 +3114,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -3091,7 +3122,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0</v>
@@ -3099,7 +3130,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -3107,7 +3138,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0</v>
@@ -3115,7 +3146,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -3123,7 +3154,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -3131,7 +3162,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0</v>
@@ -3139,7 +3170,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>0</v>
@@ -3147,7 +3178,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>0</v>
@@ -3155,7 +3186,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0</v>
@@ -3163,7 +3194,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -3171,7 +3202,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -3179,7 +3210,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0</v>
@@ -3187,7 +3218,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -3195,7 +3226,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>0</v>
@@ -3203,7 +3234,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0</v>
@@ -3211,7 +3242,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0</v>
@@ -3219,7 +3250,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>0</v>
@@ -3227,7 +3258,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -3235,7 +3266,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0</v>
@@ -3243,7 +3274,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0</v>
@@ -3251,7 +3282,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0</v>
@@ -3259,7 +3290,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>
@@ -3267,7 +3298,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>0</v>
@@ -3275,7 +3306,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>0</v>
@@ -3283,7 +3314,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0</v>
@@ -3291,7 +3322,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -3299,7 +3330,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>0</v>
@@ -3307,7 +3338,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>0</v>
@@ -3315,7 +3346,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>0</v>
@@ -3323,7 +3354,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>0</v>
@@ -3331,7 +3362,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0</v>
@@ -3339,7 +3370,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>0</v>
@@ -3347,7 +3378,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>0</v>
@@ -3355,7 +3386,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -3363,7 +3394,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>0</v>
@@ -3372,7 +3403,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3387,13 +3418,13 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,24 +3443,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3444,133 +3475,132 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3585,133 +3615,132 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3726,731 +3755,730 @@
   </sheetPr>
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B1" s="16"/>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4463,85 +4491,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AV8"/>
+  <dimension ref="A1:AW8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="9.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="26" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="47" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="49" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="0"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
-      <c r="I1" s="0"/>
+      <c r="H1" s="0"/>
       <c r="J1" s="0"/>
-      <c r="AS1" s="0"/>
+      <c r="K1" s="0"/>
       <c r="AT1" s="0"/>
       <c r="AU1" s="0"/>
       <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="0"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
-      <c r="I2" s="0"/>
+      <c r="H2" s="0"/>
       <c r="J2" s="0"/>
-      <c r="AS2" s="0"/>
+      <c r="K2" s="0"/>
       <c r="AT2" s="0"/>
       <c r="AU2" s="0"/>
       <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
     </row>
     <row r="4" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -4563,6 +4602,7 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
@@ -4571,7 +4611,7 @@
       <c r="B5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -4640,115 +4680,123 @@
       <c r="Y5" s="13" t="s">
         <v>59</v>
       </c>
+      <c r="Z5" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="16" t="s">
         <v>62</v>
       </c>
+      <c r="C6" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="D6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="17" t="s">
         <v>64</v>
       </c>
+      <c r="E6" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="F6" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>68</v>
       </c>
+      <c r="I6" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="J6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="16" t="s">
         <v>70</v>
       </c>
+      <c r="K6" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="L6" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="X6" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Y6" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>88</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="6" t="n">
+        <v>89</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="18" t="n">
+      <c r="G7" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="H7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="19"/>
       <c r="J7" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="M7" s="19"/>
+      <c r="L7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
@@ -4780,93 +4828,97 @@
       <c r="AP7" s="19"/>
       <c r="AQ7" s="19"/>
       <c r="AR7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AS7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="6" t="n">
+      <c r="F8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="6" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="H8" s="6" t="n">
         <v>0</v>
       </c>
       <c r="J8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:Y4"/>
+    <mergeCell ref="D4:Z4"/>
   </mergeCells>
   <dataValidations count="12">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O7:P8" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P7:Q8" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W8 Y7:Y8" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:X8 Z7:Z8" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L8" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M7:M8" type="list">
       <formula1>validation_choices</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K7:K8" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L7:L8" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:G8 I7:J8 N7:N8 Q7:R8" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G7:H8 J7:K8 O7:O8 R7:S8" type="list">
       <formula1>boolean_choices</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M7" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N7" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S7" type="decimal">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T7" type="decimal">
       <formula1>$O$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C8" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D8" type="list">
       <formula1>attribute_types</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D8" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E8" type="list">
       <formula1>attribute_groups</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U7:U8" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V7:V8" type="list">
       <formula1>metric_types</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V7:V8" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W7:W8" type="list">
       <formula1>metric_units</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4880,32 +4932,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="1:7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="8" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="27" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1000" min="998" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1001" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="997" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1021" min="1001" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4913,6 +4965,9 @@
       <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="W1" s="0"/>
       <c r="X1" s="0"/>
       <c r="Y1" s="0"/>
@@ -4920,16 +4975,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
@@ -4940,7 +4998,7 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="ALM3" s="0"/>
       <c r="ALN3" s="0"/>
@@ -4972,24 +5030,24 @@
         <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="18" t="n">
         <v>1</v>
@@ -5016,7 +5074,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -5038,7 +5096,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5052,32 +5110,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="8" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="7" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="27" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1000" min="998" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1001" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="997" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1021" min="1001" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5085,6 +5143,9 @@
       <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="W1" s="0"/>
       <c r="X1" s="0"/>
       <c r="Y1" s="0"/>
@@ -5092,16 +5153,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
@@ -5112,7 +5176,7 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="ALM3" s="0"/>
       <c r="ALN3" s="0"/>
@@ -5144,24 +5208,24 @@
         <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="18" t="n">
         <v>1</v>
@@ -5199,7 +5263,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5213,80 +5277,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D2" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="19" t="n">
+      <c r="A4" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="C4" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
+      <c r="C5" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5301,20 +5380,20 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -5326,7 +5405,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -5334,13 +5413,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -5349,7 +5428,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5365,24 +5444,23 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="6" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -5391,53 +5469,53 @@
     </row>
     <row r="2" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -5452,7 +5530,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5467,56 +5545,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>125</v>
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5531,7 +5621,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5547,34 +5637,34 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -5582,7 +5672,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -5600,7 +5690,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fix EE init fixtures labels
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal_EE/init.xlsx
+++ b/src/Resources/fixtures/minimal_EE/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="410">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -1779,9 +1779,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1791,7 +1791,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9933840" cy="9532080"/>
+          <a:ext cx="9828720" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1824,9 +1824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1836,7 +1836,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9933840" cy="9532080"/>
+          <a:ext cx="9828720" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1869,9 +1869,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1881,7 +1881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9933840" cy="9532080"/>
+          <a:ext cx="9828720" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1919,9 +1919,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
+      <xdr:colOff>275400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1931,7 +1931,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9924480" cy="9532080"/>
+          <a:ext cx="9800280" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1969,9 +1969,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>456840</xdr:colOff>
+      <xdr:colOff>456480</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1981,7 +1981,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9924480" cy="9532080"/>
+          <a:ext cx="9810000" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2018,8 +2018,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>325800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>325440</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
@@ -2031,7 +2031,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6007320" cy="9529560"/>
+          <a:ext cx="7362000" cy="9868680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2040,7 +2040,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2060,8 +2060,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>325800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>325440</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
@@ -2073,7 +2073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6007320" cy="9529560"/>
+          <a:ext cx="7362000" cy="9868680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2082,7 +2082,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2108,9 +2108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>78480</xdr:colOff>
+      <xdr:colOff>78120</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2120,7 +2120,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6826680" cy="10387440"/>
+          <a:ext cx="6759720" cy="10387080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2129,7 +2129,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2150,9 +2150,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>78480</xdr:colOff>
+      <xdr:colOff>78120</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2162,7 +2162,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="6826680" cy="10387440"/>
+          <a:ext cx="6759720" cy="10387080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2171,7 +2171,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2192,9 +2192,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>104400</xdr:colOff>
+      <xdr:colOff>104040</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2204,7 +2204,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11000880" cy="9732240"/>
+          <a:ext cx="10866960" cy="9731880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2237,9 +2237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>104400</xdr:colOff>
+      <xdr:colOff>104040</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2249,7 +2249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11000880" cy="9732240"/>
+          <a:ext cx="10866960" cy="9731880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2287,9 +2287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>326160</xdr:colOff>
+      <xdr:colOff>325800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2299,7 +2299,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="10979640" cy="9829800"/>
+          <a:ext cx="10836360" cy="9829440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2308,7 +2308,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2329,9 +2329,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>326160</xdr:colOff>
+      <xdr:colOff>325800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2341,7 +2341,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="81000" y="0"/>
-          <a:ext cx="10979640" cy="9829800"/>
+          <a:ext cx="10836360" cy="9829440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2350,7 +2350,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2378,8 +2378,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,17 +2563,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="21.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2584,21 +2583,28 @@
       <c r="B1" s="25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>62</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2608,34 +2614,38 @@
       <c r="B4" s="32" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="31"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="31"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
         <v>146</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>147</v>
       </c>
+      <c r="C7" s="31"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:C4" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2663,7 +2673,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,25 +2737,25 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="16" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>158</v>
       </c>
@@ -2785,21 +2797,16 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,15 +2903,15 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R41" activeCellId="0" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.16326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,9 +3753,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -3804,9 +3808,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,9 +3949,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4086,9 +4090,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,36 +4829,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5256,25 +5257,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="997" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1000" min="998" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1021" min="1001" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1000" min="998" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5412,25 +5412,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="997" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1000" min="998" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1021" min="1001" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1000" min="998" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5557,11 +5556,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5649,17 +5647,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO2" activeCellId="0" sqref="AO2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.515306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5670,8 +5669,9 @@
       <c r="C1" s="25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
         <v>35</v>
       </c>
@@ -5681,8 +5681,11 @@
       <c r="C2" s="26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>115</v>
       </c>
@@ -5691,6 +5694,9 @@
       </c>
       <c r="C3" s="26" t="s">
         <v>62</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -5715,20 +5721,19 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5834,11 +5839,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5919,14 +5923,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>